<commit_message>
basic performance summary with job data.
</commit_message>
<xml_diff>
--- a/app/performance_summary_table_schema.xlsx
+++ b/app/performance_summary_table_schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cantec3403-my.sharepoint.com/personal/j_sullivan-phillips_cantec_ca/Documents/Desktop/CSC/Schedule Assist/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_F25DC773A252ABDACC1048E1315E42F05ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1AC1618E-E6B8-4B6B-B0E5-618D6C2E809F}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="11_F25DC773A252ABDACC1048E1315E42F05ADE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77200604-E281-4C03-B1AC-CAC90ABCB97A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,36 +25,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>jobType</t>
-  </si>
-  <si>
-    <t>jobId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>address</t>
   </si>
   <si>
-    <t>customerName</t>
-  </si>
-  <si>
-    <t>jobStatus</t>
-  </si>
-  <si>
-    <t>scheduledDate</t>
-  </si>
-  <si>
-    <t>completedOn</t>
-  </si>
-  <si>
     <t>revenue</t>
   </si>
   <si>
-    <t>invoiceStatus</t>
-  </si>
-  <si>
-    <t>onSiteHours</t>
+    <t>TABLE 1</t>
+  </si>
+  <si>
+    <t>TABLE 2: job_clock_events</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>job_id</t>
+  </si>
+  <si>
+    <t>tech_name</t>
+  </si>
+  <si>
+    <t>hours</t>
+  </si>
+  <si>
+    <t>job_type</t>
+  </si>
+  <si>
+    <t>customer_name</t>
+  </si>
+  <si>
+    <t>job_status</t>
+  </si>
+  <si>
+    <t>scheduled_date</t>
+  </si>
+  <si>
+    <t>completed_on</t>
+  </si>
+  <si>
+    <t>on_site_hours</t>
   </si>
 </sst>
 </file>
@@ -372,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="B10" sqref="B10:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -383,36 +395,57 @@
     <col min="1" max="21" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D5" t="s">
         <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>